<commit_message>
change panelist selector toolwith Gemini AI
</commit_message>
<xml_diff>
--- a/panel_member_info.xlsx
+++ b/panel_member_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\mcp-ai-tools-suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DE294F-E52A-469F-8DC6-99528DA92A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56341201-B1DB-4C28-86B9-31F488B9BFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,105 +25,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
-  <si>
-    <t>Panel Member</t>
-  </si>
-  <si>
-    <t>Primary Skill</t>
-  </si>
-  <si>
-    <t>Secondary Skill</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t>Django</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>Spring Boot</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>Machine Learning</t>
-  </si>
-  <si>
-    <t>Deep Learning</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>DevOps</t>
-  </si>
-  <si>
-    <t>Kubernetes</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>UI/UX Design</t>
-  </si>
-  <si>
-    <t>Graphic Design</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>Cloud Architecture</t>
-  </si>
-  <si>
-    <t>AWS</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>Cybersecurity</t>
-  </si>
-  <si>
-    <t>Network Security</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>Data Engineering</t>
-  </si>
-  <si>
-    <t>SQL</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>Product Management</t>
-  </si>
-  <si>
-    <t>Agile Methodology</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>ReactJS</t>
-  </si>
-  <si>
-    <t>Node.js</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Experience (Years)</t>
+  </si>
+  <si>
+    <t>Available Now</t>
+  </si>
+  <si>
+    <t>Ananya Rao</t>
+  </si>
+  <si>
+    <t>Python, ML, SQL</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Ravi Kumar</t>
+  </si>
+  <si>
+    <t>Java, Spring, System Design</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Shruti Nair</t>
+  </si>
+  <si>
+    <t>Python, AI, Deep Learning</t>
+  </si>
+  <si>
+    <t>Vikram Patil</t>
+  </si>
+  <si>
+    <t>.NET, C#, Azure</t>
+  </si>
+  <si>
+    <t>Leela Sinha</t>
+  </si>
+  <si>
+    <t>Python, Django, REST APIs</t>
+  </si>
+  <si>
+    <t>Arun Menon</t>
+  </si>
+  <si>
+    <t>JavaScript, React, Node.js</t>
+  </si>
+  <si>
+    <t>Divya Shetty</t>
+  </si>
+  <si>
+    <t>Data Science, R, Python</t>
+  </si>
+  <si>
+    <t>Mohan Das</t>
+  </si>
+  <si>
+    <t>DevOps, AWS, Terraform</t>
+  </si>
+  <si>
+    <t>Kiran Bhandari</t>
+  </si>
+  <si>
+    <t>Java, Kotlin, Microservices</t>
+  </si>
+  <si>
+    <t>Tara Desai</t>
+  </si>
+  <si>
+    <t>Python, NLP, Transformers</t>
   </si>
 </sst>
 </file>
@@ -455,20 +434,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,115 +458,148 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C9" s="2">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="C10" s="2">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>32</v>
+      <c r="C11" s="2">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>